<commit_message>
Updated data for traces 2&3
</commit_message>
<xml_diff>
--- a/project2/experiment_results_excel.xlsx
+++ b/project2/experiment_results_excel.xlsx
@@ -1,26 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephensnow/Documents/COE1541/projects1541/project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Nick\1541\proj2\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="15960" windowHeight="17480"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="15960" windowHeight="17475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="exp1" sheetId="1" r:id="rId1"/>
     <sheet name="exp2" sheetId="2" r:id="rId2"/>
     <sheet name="exp3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="27">
   <si>
     <t>Table 1</t>
   </si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>sample_large3</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Table 3</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -319,6 +322,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -326,6 +332,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -406,6 +418,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -424,10 +439,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.151767"/>
+          <c:x val="0.15176700000000001"/>
           <c:y val="0.126667"/>
-          <c:w val="0.843233"/>
-          <c:h val="0.809167"/>
+          <c:w val="0.84323300000000001"/>
+          <c:h val="0.80916699999999997"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -483,13 +498,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.023845511E9</c:v>
+                  <c:v>1023845511</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.76070403E8</c:v>
+                  <c:v>576070403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.61561179E8</c:v>
+                  <c:v>561561179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,13 +559,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.698781999E9</c:v>
+                  <c:v>3698781999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.562773747E9</c:v>
+                  <c:v>3562773747</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.557251525E9</c:v>
+                  <c:v>3557251525</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,13 +620,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.425636583E9</c:v>
+                  <c:v>1425636583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.135372173E9</c:v>
+                  <c:v>1135372173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.087482979E9</c:v>
+                  <c:v>1087482979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,11 +642,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="-10"/>
-        <c:axId val="401615680"/>
-        <c:axId val="401617728"/>
+        <c:axId val="204484616"/>
+        <c:axId val="204481088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="401615680"/>
+        <c:axId val="204484616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,7 +680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401617728"/>
+        <c:crossAx val="204481088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -673,7 +688,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="401617728"/>
+        <c:axId val="204481088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,11 +731,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401615680"/>
+        <c:crossAx val="204484616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0E9"/>
-        <c:minorUnit val="5.0E8"/>
+        <c:majorUnit val="1000000000"/>
+        <c:minorUnit val="500000000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -737,10 +752,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13426"/>
-          <c:y val="0.0"/>
-          <c:w val="0.820175"/>
-          <c:h val="0.065"/>
+          <c:x val="0.13425999999999999"/>
+          <c:y val="0"/>
+          <c:w val="0.82017499999999999"/>
+          <c:h val="6.5000000000000002E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1926,65 +1941,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="16.33203125" style="1" customWidth="1"/>
-    <col min="14" max="256" width="16.33203125" customWidth="1"/>
+    <col min="1" max="13" width="16.28515625" style="1" customWidth="1"/>
+    <col min="14" max="256" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="18" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -2025,7 +2040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -2069,7 +2084,7 @@
         <v>806793489</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -2113,7 +2128,7 @@
         <v>477913189</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -2157,7 +2172,7 @@
         <v>379071289</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -2201,7 +2216,7 @@
         <v>354810089</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -2216,112 +2231,264 @@
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-    </row>
-    <row r="16" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+    </row>
+    <row r="10" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
+        <v>21979534</v>
+      </c>
+      <c r="C12" s="9">
+        <v>14105451</v>
+      </c>
+      <c r="D12" s="10">
+        <f>B12/(B12+C12)</f>
+        <v>0.60910470102731096</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2892582589</v>
+      </c>
+      <c r="F12" s="9">
+        <v>19281063</v>
+      </c>
+      <c r="G12" s="9">
+        <v>16803922</v>
+      </c>
+      <c r="H12" s="10">
+        <f>F12/(F12+G12)</f>
+        <v>0.53432370832355891</v>
+      </c>
+      <c r="I12" s="9">
+        <v>2552742889</v>
+      </c>
+      <c r="J12" s="9">
+        <v>16801397</v>
+      </c>
+      <c r="K12" s="9">
+        <v>19283588</v>
+      </c>
+      <c r="L12" s="10">
+        <f>J12/(J12+K12)</f>
+        <v>0.46560631797408258</v>
+      </c>
+      <c r="M12" s="9">
+        <v>2249452089</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8">
+        <v>20983124</v>
+      </c>
+      <c r="C13" s="9">
+        <v>15101861</v>
+      </c>
+      <c r="D13" s="10">
+        <f>B13/(B13+C13)</f>
+        <v>0.58149183102057544</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2729053289</v>
+      </c>
+      <c r="F13" s="9">
+        <v>19401995</v>
+      </c>
+      <c r="G13" s="9">
+        <v>16682990</v>
+      </c>
+      <c r="H13" s="10">
+        <f>F13/(F13+G13)</f>
+        <v>0.53767501912499061</v>
+      </c>
+      <c r="I13" s="9">
+        <v>2548892989</v>
+      </c>
+      <c r="J13" s="9">
+        <v>17028949</v>
+      </c>
+      <c r="K13" s="9">
+        <v>19056036</v>
+      </c>
+      <c r="L13" s="10">
+        <f>J13/(J13+K13)</f>
+        <v>0.47191232031827091</v>
+      </c>
+      <c r="M13" s="9">
+        <v>2267742589</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
+        <v>19431866</v>
+      </c>
+      <c r="C14" s="9">
+        <v>16653119</v>
+      </c>
+      <c r="D14" s="10">
+        <f>B14/(B14+C14)</f>
+        <v>0.53850281495198071</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2543916889</v>
+      </c>
+      <c r="F14" s="9">
+        <v>16231800</v>
+      </c>
+      <c r="G14" s="9">
+        <v>19853185</v>
+      </c>
+      <c r="H14" s="10">
+        <f>F14/(F14+G14)</f>
+        <v>0.44982144235337773</v>
+      </c>
+      <c r="I14" s="9">
+        <v>2188924689</v>
+      </c>
+      <c r="J14" s="9">
+        <v>15108316</v>
+      </c>
+      <c r="K14" s="9">
+        <v>20976669</v>
+      </c>
+      <c r="L14" s="10">
+        <f>J14/(J14+K14)</f>
+        <v>0.41868705224624592</v>
+      </c>
+      <c r="M14" s="9">
+        <v>2052171789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
+        <v>18781477</v>
+      </c>
+      <c r="C15" s="9">
+        <v>17303508</v>
+      </c>
+      <c r="D15" s="10">
+        <f>B15/(B15+C15)</f>
+        <v>0.52047900255466362</v>
+      </c>
+      <c r="E15" s="9">
+        <v>2262377589</v>
+      </c>
+      <c r="F15" s="9">
+        <v>8746736</v>
+      </c>
+      <c r="G15" s="9">
+        <v>27338249</v>
+      </c>
+      <c r="H15" s="10">
+        <f>F15/(F15+G15)</f>
+        <v>0.24239267385035632</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1131601689</v>
+      </c>
+      <c r="J15" s="9">
+        <v>7884832</v>
+      </c>
+      <c r="K15" s="9">
+        <v>28200153</v>
+      </c>
+      <c r="L15" s="10">
+        <f>J15/(J15+K15)</f>
+        <v>0.21850728218398871</v>
+      </c>
+      <c r="M15" s="9">
+        <v>1024405189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -2336,117 +2503,277 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-    </row>
-    <row r="21" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-    </row>
-    <row r="23" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+    <row r="17" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8">
+        <v>14522563</v>
+      </c>
+      <c r="C20" s="9">
+        <v>21246983</v>
+      </c>
+      <c r="D20" s="10">
+        <f>B20/(B20+C20)</f>
+        <v>0.40600355956432882</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1932011589</v>
+      </c>
+      <c r="F20" s="9">
+        <v>5376131</v>
+      </c>
+      <c r="G20" s="9">
+        <v>30393415</v>
+      </c>
+      <c r="H20" s="10">
+        <f>F20/(F20+G20)</f>
+        <v>0.15029911198761092</v>
+      </c>
+      <c r="I20" s="9">
+        <v>736741489</v>
+      </c>
+      <c r="J20" s="9">
+        <v>2616389</v>
+      </c>
+      <c r="K20" s="9">
+        <v>33153157</v>
+      </c>
+      <c r="L20" s="10">
+        <f>J20/(J20+K20)</f>
+        <v>7.3145714513681556E-2</v>
+      </c>
+      <c r="M20" s="9">
+        <v>411360589</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="8">
+        <v>13901379</v>
+      </c>
+      <c r="C21" s="9">
+        <v>21868167</v>
+      </c>
+      <c r="D21" s="10">
+        <f>B21/(B21+C21)</f>
+        <v>0.38863727820308369</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1736361689</v>
+      </c>
+      <c r="F21" s="9">
+        <v>5022055</v>
+      </c>
+      <c r="G21" s="9">
+        <v>30747491</v>
+      </c>
+      <c r="H21" s="10">
+        <f>F21/(F21+G21)</f>
+        <v>0.14040030030014919</v>
+      </c>
+      <c r="I21" s="9">
+        <v>647186089</v>
+      </c>
+      <c r="J21" s="9">
+        <v>2009319</v>
+      </c>
+      <c r="K21" s="9">
+        <v>33760227</v>
+      </c>
+      <c r="L21" s="10">
+        <f>J21/(J21+K21)</f>
+        <v>5.6174014621264694E-2</v>
+      </c>
+      <c r="M21" s="9">
+        <v>316472689</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="8">
+        <v>14570698</v>
+      </c>
+      <c r="C22" s="9">
+        <v>21198848</v>
+      </c>
+      <c r="D22" s="10">
+        <f>B22/(B22+C22)</f>
+        <v>0.40734925738224353</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1783214789</v>
+      </c>
+      <c r="F22" s="9">
+        <v>4939452</v>
+      </c>
+      <c r="G22" s="9">
+        <v>30830094</v>
+      </c>
+      <c r="H22" s="10">
+        <f>F22/(F22+G22)</f>
+        <v>0.13809098946908635</v>
+      </c>
+      <c r="I22" s="9">
+        <v>626084289</v>
+      </c>
+      <c r="J22" s="9">
+        <v>1595973</v>
+      </c>
+      <c r="K22" s="9">
+        <v>34173573</v>
+      </c>
+      <c r="L22" s="10">
+        <f>J22/(J22+K22)</f>
+        <v>4.4618206784061504E-2</v>
+      </c>
+      <c r="M22" s="9">
+        <v>262615689</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="8">
+        <v>17098511</v>
+      </c>
+      <c r="C23" s="9">
+        <v>18671035</v>
+      </c>
+      <c r="D23" s="10">
+        <f>B23/(B23+C23)</f>
+        <v>0.47801867543971621</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2092121689</v>
+      </c>
+      <c r="F23" s="9">
+        <v>5611154</v>
+      </c>
+      <c r="G23" s="9">
+        <v>30158392</v>
+      </c>
+      <c r="H23" s="10">
+        <f>F23/(F23+G23)</f>
+        <v>0.15686958956649882</v>
+      </c>
+      <c r="I23" s="9">
+        <v>706401289</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1562525</v>
+      </c>
+      <c r="K23" s="9">
+        <v>34207021</v>
+      </c>
+      <c r="L23" s="10">
+        <f>J23/(J23+K23)</f>
+        <v>4.3683109648637981E-2</v>
+      </c>
+      <c r="M23" s="9">
+        <v>257811189</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="A17:M17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="J18:M18"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A9:M9"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
@@ -2458,60 +2785,1202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="22" width="16.28515625" style="14" customWidth="1"/>
+    <col min="23" max="256" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+    </row>
+    <row r="2" spans="1:22" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8">
+        <v>10959701</v>
+      </c>
+      <c r="C3" s="9">
+        <v>19479164</v>
+      </c>
+      <c r="D3" s="10">
+        <f>B3/(B3+C3)</f>
+        <v>0.36005616503769111</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2005538</v>
+      </c>
+      <c r="F3" s="9">
+        <v>8954163</v>
+      </c>
+      <c r="G3" s="10">
+        <f>E3/(E3+F3)</f>
+        <v>0.18299203600536182</v>
+      </c>
+      <c r="H3" s="9">
+        <v>807395307</v>
+      </c>
+      <c r="I3" s="9">
+        <v>7881980</v>
+      </c>
+      <c r="J3" s="9">
+        <v>22556885</v>
+      </c>
+      <c r="K3" s="10">
+        <f>I3/(I3+J3)</f>
+        <v>0.25894460913703582</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1878723</v>
+      </c>
+      <c r="M3" s="9">
+        <v>6003257</v>
+      </c>
+      <c r="N3" s="10">
+        <f>L3/(L3+M3)</f>
+        <v>0.23835673269914412</v>
+      </c>
+      <c r="O3" s="9">
+        <v>699632217</v>
+      </c>
+      <c r="P3" s="9">
+        <v>5546272</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>24892593</v>
+      </c>
+      <c r="R3" s="10">
+        <f>P3/(P3+Q3)</f>
+        <v>0.18221021053183159</v>
+      </c>
+      <c r="S3" s="9">
+        <v>1758416</v>
+      </c>
+      <c r="T3" s="9">
+        <v>3787856</v>
+      </c>
+      <c r="U3" s="10">
+        <f>S3/(S3+T3)</f>
+        <v>0.31704467433259675</v>
+      </c>
+      <c r="V3" s="9">
+        <v>621756731</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8">
+        <v>9482452</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20956413</v>
+      </c>
+      <c r="D4" s="10">
+        <f>B4/(B4+C4)</f>
+        <v>0.31152449343955502</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1942742</v>
+      </c>
+      <c r="F4" s="9">
+        <v>8539710</v>
+      </c>
+      <c r="G4" s="10">
+        <f>E4/(E4+F4)</f>
+        <v>0.18533278282600293</v>
+      </c>
+      <c r="H4" s="9">
+        <v>670320319</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5508413</v>
+      </c>
+      <c r="J4" s="9">
+        <v>24930452</v>
+      </c>
+      <c r="K4" s="10">
+        <f>I4/(I4+J4)</f>
+        <v>0.18096643879461341</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1549586</v>
+      </c>
+      <c r="M4" s="9">
+        <v>3958827</v>
+      </c>
+      <c r="N4" s="10">
+        <f>L4/(L4+M4)</f>
+        <v>0.28131260310365253</v>
+      </c>
+      <c r="O4" s="9">
+        <v>452482203</v>
+      </c>
+      <c r="P4" s="9">
+        <v>3240984</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>27197881</v>
+      </c>
+      <c r="R4" s="10">
+        <f>P4/(P4+Q4)</f>
+        <v>0.10647519215976023</v>
+      </c>
+      <c r="S4" s="9">
+        <v>1483241</v>
+      </c>
+      <c r="T4" s="9">
+        <v>1757743</v>
+      </c>
+      <c r="U4" s="10">
+        <f>S4/(S4+T4)</f>
+        <v>0.45765144166092769</v>
+      </c>
+      <c r="V4" s="9">
+        <v>387888813</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8">
+        <v>14779659</v>
+      </c>
+      <c r="C5" s="9">
+        <v>15659206</v>
+      </c>
+      <c r="D5" s="10">
+        <f>B5/(B5+C5)</f>
+        <v>0.48555223724669105</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1474528</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3428571</v>
+      </c>
+      <c r="G5" s="10">
+        <f>E5/(E5+F5)</f>
+        <v>0.30073388279535046</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1184781011</v>
+      </c>
+      <c r="I5" s="9">
+        <v>4903099</v>
+      </c>
+      <c r="J5" s="9">
+        <v>25535766</v>
+      </c>
+      <c r="K5" s="10">
+        <f>I5/(I5+J5)</f>
+        <v>0.16108021767565905</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1474537</v>
+      </c>
+      <c r="M5" s="9">
+        <v>3428562</v>
+      </c>
+      <c r="N5" s="10">
+        <f>L5/(L5+M5)</f>
+        <v>0.30073571836913754</v>
+      </c>
+      <c r="O5" s="9">
+        <v>389759891</v>
+      </c>
+      <c r="P5" s="9">
+        <v>2526847</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>27912018</v>
+      </c>
+      <c r="R5" s="10">
+        <f>P5/(P5+Q5)</f>
+        <v>8.301383773672244E-2</v>
+      </c>
+      <c r="S5" s="9">
+        <v>1365113</v>
+      </c>
+      <c r="T5" s="9">
+        <v>1161734</v>
+      </c>
+      <c r="U5" s="10">
+        <f>S5/(S5+T5)</f>
+        <v>0.54024363168802858</v>
+      </c>
+      <c r="V5" s="9">
+        <v>311524099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8">
+        <v>20443432</v>
+      </c>
+      <c r="C6" s="9">
+        <v>9995433</v>
+      </c>
+      <c r="D6" s="10">
+        <f>B6/(B6+C6)</f>
+        <v>0.67162267712675883</v>
+      </c>
+      <c r="E6" s="9">
+        <v>4663156</v>
+      </c>
+      <c r="F6" s="9">
+        <v>15780276</v>
+      </c>
+      <c r="G6" s="10">
+        <f>E6/(E6+F6)</f>
+        <v>0.22810044810479962</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1970341931</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5176439</v>
+      </c>
+      <c r="J6" s="9">
+        <v>25262426</v>
+      </c>
+      <c r="K6" s="10">
+        <f>I6/(I6+J6)</f>
+        <v>0.17006018456995686</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1515819</v>
+      </c>
+      <c r="M6" s="9">
+        <v>3660620</v>
+      </c>
+      <c r="N6" s="10">
+        <f>L6/(L6+M6)</f>
+        <v>0.29283045738585928</v>
+      </c>
+      <c r="O6" s="9">
+        <v>412603543</v>
+      </c>
+      <c r="P6" s="9">
+        <v>2351529</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>28087336</v>
+      </c>
+      <c r="R6" s="10">
+        <f>P6/(P6+Q6)</f>
+        <v>7.7254161743547267E-2</v>
+      </c>
+      <c r="S6" s="9">
+        <v>1324996</v>
+      </c>
+      <c r="T6" s="9">
+        <v>1026533</v>
+      </c>
+      <c r="U6" s="10">
+        <f>S6/(S6+T6)</f>
+        <v>0.56346147549105285</v>
+      </c>
+      <c r="V6" s="9">
+        <v>291782827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="13"/>
+    </row>
+    <row r="8" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="13"/>
+    </row>
+    <row r="9" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="12">
+        <v>21979534</v>
+      </c>
+      <c r="C9" s="13">
+        <v>14105451</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" ref="D8:D18" si="0">B9/(B9+C9)</f>
+        <v>0.60910470102731096</v>
+      </c>
+      <c r="E9" s="13">
+        <v>10474237</v>
+      </c>
+      <c r="F9" s="13">
+        <v>11505297</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" ref="G8:G18" si="1">E9/(E9+F9)</f>
+        <v>0.47654499863372901</v>
+      </c>
+      <c r="H9" s="13">
+        <v>2829654277</v>
+      </c>
+      <c r="I9" s="13">
+        <v>19281063</v>
+      </c>
+      <c r="J9" s="13">
+        <v>16803922</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" ref="K8:K18" si="2">I9/(I9+J9)</f>
+        <v>0.53432370832355891</v>
+      </c>
+      <c r="L9" s="13">
+        <v>9780768</v>
+      </c>
+      <c r="M9" s="13">
+        <v>9500295</v>
+      </c>
+      <c r="N9" s="10">
+        <f t="shared" ref="N8:N18" si="3">L9/(L9+M9)</f>
+        <v>0.50727327637485542</v>
+      </c>
+      <c r="O9" s="13">
+        <v>2579861895</v>
+      </c>
+      <c r="P9" s="13">
+        <v>16801397</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>19283588</v>
+      </c>
+      <c r="R9" s="10">
+        <f t="shared" ref="R8:R18" si="4">P9/(P9+Q9)</f>
+        <v>0.46560631797408258</v>
+      </c>
+      <c r="S9" s="13">
+        <v>7899635</v>
+      </c>
+      <c r="T9" s="13">
+        <v>8901762</v>
+      </c>
+      <c r="U9" s="10">
+        <f t="shared" ref="U8:U18" si="5">S9/(S9+T9)</f>
+        <v>0.47017727156854872</v>
+      </c>
+      <c r="V9" s="13">
+        <v>2127646447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="12">
+        <v>20983124</v>
+      </c>
+      <c r="C10" s="13">
+        <v>15101861</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="0"/>
+        <v>0.58149183102057544</v>
+      </c>
+      <c r="E10" s="13">
+        <v>16220037</v>
+      </c>
+      <c r="F10" s="13">
+        <v>4763087</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.77300391495565679</v>
+      </c>
+      <c r="H10" s="13">
+        <v>3316265319</v>
+      </c>
+      <c r="I10" s="13">
+        <v>19401995</v>
+      </c>
+      <c r="J10" s="13">
+        <v>16682990</v>
+      </c>
+      <c r="K10" s="10">
+        <f t="shared" si="2"/>
+        <v>0.53767501912499061</v>
+      </c>
+      <c r="L10" s="13">
+        <v>14851097</v>
+      </c>
+      <c r="M10" s="13">
+        <v>4550898</v>
+      </c>
+      <c r="N10" s="10">
+        <f t="shared" si="3"/>
+        <v>0.76544174967574208</v>
+      </c>
+      <c r="O10" s="13">
+        <v>3107700701</v>
+      </c>
+      <c r="P10" s="13">
+        <v>17028949</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>19056036</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" si="4"/>
+        <v>0.47191232031827091</v>
+      </c>
+      <c r="S10" s="13">
+        <v>12709453</v>
+      </c>
+      <c r="T10" s="13">
+        <v>4319496</v>
+      </c>
+      <c r="U10" s="10">
+        <f t="shared" si="5"/>
+        <v>0.74634394641736257</v>
+      </c>
+      <c r="V10" s="13">
+        <v>2753234577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12">
+        <v>19431866</v>
+      </c>
+      <c r="C11" s="13">
+        <v>16653119</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.53850281495198071</v>
+      </c>
+      <c r="E11" s="13">
+        <v>17078701</v>
+      </c>
+      <c r="F11" s="13">
+        <v>2353165</v>
+      </c>
+      <c r="G11" s="10">
+        <f t="shared" si="1"/>
+        <v>0.87890174829324164</v>
+      </c>
+      <c r="H11" s="13">
+        <v>3341260435</v>
+      </c>
+      <c r="I11" s="13">
+        <v>16231800</v>
+      </c>
+      <c r="J11" s="13">
+        <v>19853185</v>
+      </c>
+      <c r="K11" s="10">
+        <f t="shared" si="2"/>
+        <v>0.44982144235337773</v>
+      </c>
+      <c r="L11" s="13">
+        <v>14277529</v>
+      </c>
+      <c r="M11" s="13">
+        <v>1954271</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" si="3"/>
+        <v>0.87960232383346271</v>
+      </c>
+      <c r="O11" s="13">
+        <v>2943627903</v>
+      </c>
+      <c r="P11" s="13">
+        <v>15108316</v>
+      </c>
+      <c r="Q11" s="13">
+        <v>20976669</v>
+      </c>
+      <c r="R11" s="10">
+        <f t="shared" si="4"/>
+        <v>0.41868705224624592</v>
+      </c>
+      <c r="S11" s="13">
+        <v>13229109</v>
+      </c>
+      <c r="T11" s="13">
+        <v>1879207</v>
+      </c>
+      <c r="U11" s="10">
+        <f t="shared" si="5"/>
+        <v>0.87561770616923817</v>
+      </c>
+      <c r="V11" s="13">
+        <v>2761043329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12">
+        <v>18781477</v>
+      </c>
+      <c r="C12" s="13">
+        <v>17303508</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.52047900255466362</v>
+      </c>
+      <c r="E12" s="13">
+        <v>15436822</v>
+      </c>
+      <c r="F12" s="13">
+        <v>3344655</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="1"/>
+        <v>0.82191736038651275</v>
+      </c>
+      <c r="H12" s="13">
+        <v>2496135277</v>
+      </c>
+      <c r="I12" s="13">
+        <v>8746736</v>
+      </c>
+      <c r="J12" s="13">
+        <v>27338249</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24239267385035632</v>
+      </c>
+      <c r="L12" s="13">
+        <v>7909277</v>
+      </c>
+      <c r="M12" s="13">
+        <v>837459</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="3"/>
+        <v>0.90425468426164912</v>
+      </c>
+      <c r="O12" s="13">
+        <v>1376833823</v>
+      </c>
+      <c r="P12" s="13">
+        <v>7884832</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>28200153</v>
+      </c>
+      <c r="R12" s="10">
+        <f t="shared" si="4"/>
+        <v>0.21850728218398871</v>
+      </c>
+      <c r="S12" s="13">
+        <v>7149788</v>
+      </c>
+      <c r="T12" s="13">
+        <v>735044</v>
+      </c>
+      <c r="U12" s="10">
+        <f t="shared" si="5"/>
+        <v>0.90677746843559892</v>
+      </c>
+      <c r="V12" s="13">
+        <v>1235243433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="13"/>
+    </row>
+    <row r="15" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12">
+        <v>14522563</v>
+      </c>
+      <c r="C15" s="13">
+        <v>21246983</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.40600355956432882</v>
+      </c>
+      <c r="E15" s="13">
+        <v>9341726</v>
+      </c>
+      <c r="F15" s="13">
+        <v>5180837</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="1"/>
+        <v>0.64325601479573546</v>
+      </c>
+      <c r="H15" s="13">
+        <v>2066535117</v>
+      </c>
+      <c r="I15" s="13">
+        <v>5376131</v>
+      </c>
+      <c r="J15" s="13">
+        <v>30393415</v>
+      </c>
+      <c r="K15" s="10">
+        <f t="shared" si="2"/>
+        <v>0.15029911198761092</v>
+      </c>
+      <c r="L15" s="13">
+        <v>3605641</v>
+      </c>
+      <c r="M15" s="13">
+        <v>1770490</v>
+      </c>
+      <c r="N15" s="10">
+        <f t="shared" si="3"/>
+        <v>0.67067580756495704</v>
+      </c>
+      <c r="O15" s="13">
+        <v>736071111</v>
+      </c>
+      <c r="P15" s="13">
+        <v>2616389</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>33153157</v>
+      </c>
+      <c r="R15" s="10">
+        <f t="shared" si="4"/>
+        <v>7.3145714513681556E-2</v>
+      </c>
+      <c r="S15" s="13">
+        <v>1874907</v>
+      </c>
+      <c r="T15" s="13">
+        <v>741482</v>
+      </c>
+      <c r="U15" s="10">
+        <f t="shared" si="5"/>
+        <v>0.71660101001800569</v>
+      </c>
+      <c r="V15" s="13">
+        <v>434296557</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="12">
+        <v>13901379</v>
+      </c>
+      <c r="C16" s="13">
+        <v>21868167</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="0"/>
+        <v>0.38863727820308369</v>
+      </c>
+      <c r="E16" s="13">
+        <v>9084457</v>
+      </c>
+      <c r="F16" s="13">
+        <v>4816922</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.65349322538433052</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1704897123</v>
+      </c>
+      <c r="I16" s="13">
+        <v>5022055</v>
+      </c>
+      <c r="J16" s="13">
+        <v>30747491</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="2"/>
+        <v>0.14040030030014919</v>
+      </c>
+      <c r="L16" s="13">
+        <v>3479013</v>
+      </c>
+      <c r="M16" s="13">
+        <v>1543042</v>
+      </c>
+      <c r="N16" s="10">
+        <f t="shared" si="3"/>
+        <v>0.69274689345297891</v>
+      </c>
+      <c r="O16" s="13">
+        <v>593779887</v>
+      </c>
+      <c r="P16" s="13">
+        <v>2009319</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>33760227</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="4"/>
+        <v>5.6174014621264694E-2</v>
+      </c>
+      <c r="S16" s="13">
+        <v>1419017</v>
+      </c>
+      <c r="T16" s="13">
+        <v>590302</v>
+      </c>
+      <c r="U16" s="10">
+        <f t="shared" si="5"/>
+        <v>0.7062178777983984</v>
+      </c>
+      <c r="V16" s="13">
+        <v>300453983</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="12">
+        <v>14570698</v>
+      </c>
+      <c r="C17" s="13">
+        <v>21198848</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="0"/>
+        <v>0.40734925738224353</v>
+      </c>
+      <c r="E17" s="13">
+        <v>9838422</v>
+      </c>
+      <c r="F17" s="13">
+        <v>4732276</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.67521967719048193</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1739584609</v>
+      </c>
+      <c r="I17" s="13">
+        <v>4939452</v>
+      </c>
+      <c r="J17" s="13">
+        <v>30830094</v>
+      </c>
+      <c r="K17" s="10">
+        <f t="shared" si="2"/>
+        <v>0.13809098946908635</v>
+      </c>
+      <c r="L17" s="13">
+        <v>3693582</v>
+      </c>
+      <c r="M17" s="13">
+        <v>1245870</v>
+      </c>
+      <c r="N17" s="10">
+        <f t="shared" si="3"/>
+        <v>0.74777161515083046</v>
+      </c>
+      <c r="O17" s="13">
+        <v>587061679</v>
+      </c>
+      <c r="P17" s="13">
+        <v>1595973</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>34173573</v>
+      </c>
+      <c r="R17" s="10">
+        <f t="shared" si="4"/>
+        <v>4.4618206784061504E-2</v>
+      </c>
+      <c r="S17" s="13">
+        <v>1198468</v>
+      </c>
+      <c r="T17" s="13">
+        <v>397505</v>
+      </c>
+      <c r="U17" s="10">
+        <f t="shared" si="5"/>
+        <v>0.75093250324410254</v>
+      </c>
+      <c r="V17" s="13">
+        <v>245311863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="12">
+        <v>17098511</v>
+      </c>
+      <c r="C18" s="13">
+        <v>18671035</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="0"/>
+        <v>0.47801867543971621</v>
+      </c>
+      <c r="E18" s="13">
+        <v>11091137</v>
+      </c>
+      <c r="F18" s="13">
+        <v>6007374</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.64866098574314457</v>
+      </c>
+      <c r="H18" s="13">
+        <v>2017773723</v>
+      </c>
+      <c r="I18" s="13">
+        <v>5611154</v>
+      </c>
+      <c r="J18" s="13">
+        <v>30158392</v>
+      </c>
+      <c r="K18" s="10">
+        <f t="shared" si="2"/>
+        <v>0.15686958956649882</v>
+      </c>
+      <c r="L18" s="13">
+        <v>4066508</v>
+      </c>
+      <c r="M18" s="13">
+        <v>1544646</v>
+      </c>
+      <c r="N18" s="10">
+        <f t="shared" si="3"/>
+        <v>0.72471865858609474</v>
+      </c>
+      <c r="O18" s="13">
+        <v>663163299</v>
+      </c>
+      <c r="P18" s="13">
+        <v>1562525</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>34207021</v>
+      </c>
+      <c r="R18" s="10">
+        <f t="shared" si="4"/>
+        <v>4.3683109648637981E-2</v>
+      </c>
+      <c r="S18" s="13">
+        <v>1216054</v>
+      </c>
+      <c r="T18" s="13">
+        <v>346471</v>
+      </c>
+      <c r="U18" s="10">
+        <f t="shared" si="5"/>
+        <v>0.77826210780627514</v>
+      </c>
+      <c r="V18" s="13">
+        <v>244003993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="22" width="16.33203125" style="14" customWidth="1"/>
-    <col min="23" max="256" width="16.33203125" customWidth="1"/>
+    <col min="1" max="22" width="16.28515625" style="15" customWidth="1"/>
+    <col min="23" max="256" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-    </row>
-    <row r="2" spans="1:22" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
+    <row r="1" spans="1:22" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+    </row>
+    <row r="2" spans="1:22" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
       <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
@@ -2576,303 +4045,253 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B3" s="8">
-        <v>10959701</v>
+        <v>9667308</v>
       </c>
       <c r="C3" s="9">
-        <v>19479164</v>
+        <v>20771557</v>
       </c>
       <c r="D3" s="10">
         <f>B3/(B3+C3)</f>
-        <v>0.36005616503769111</v>
+        <v>0.31759751882995635</v>
       </c>
       <c r="E3" s="9">
-        <v>2005579</v>
+        <v>3952546</v>
       </c>
       <c r="F3" s="9">
-        <v>8954122</v>
+        <v>5714762</v>
       </c>
       <c r="G3" s="10">
         <f>E3/(E3+F3)</f>
-        <v>0.18299577698333194</v>
+        <v>0.4088569434220985</v>
       </c>
       <c r="H3" s="9">
-        <v>807399307</v>
+        <v>1023845511</v>
       </c>
       <c r="I3" s="9">
-        <v>7881980</v>
+        <v>6514006</v>
       </c>
       <c r="J3" s="9">
-        <v>22556885</v>
+        <v>23924859</v>
       </c>
       <c r="K3" s="10">
         <f>I3/(I3+J3)</f>
-        <v>0.25894460913703582</v>
+        <v>0.21400292027971476</v>
       </c>
       <c r="L3" s="9">
-        <v>1878761</v>
+        <v>2358181</v>
       </c>
       <c r="M3" s="9">
-        <v>6003219</v>
+        <v>4155825</v>
       </c>
       <c r="N3" s="10">
         <f>L3/(L3+M3)</f>
-        <v>0.23836155382277041</v>
+        <v>0.36201701380072415</v>
       </c>
       <c r="O3" s="9">
-        <v>699636017</v>
+        <v>576070403</v>
       </c>
       <c r="P3" s="9">
-        <v>5546272</v>
+        <v>6338281</v>
       </c>
       <c r="Q3" s="9">
-        <v>24892593</v>
+        <v>24100584</v>
       </c>
       <c r="R3" s="10">
         <f>P3/(P3+Q3)</f>
-        <v>0.18221021053183159</v>
+        <v>0.2082298732229339</v>
       </c>
       <c r="S3" s="9">
-        <v>1758398</v>
+        <v>2302499</v>
       </c>
       <c r="T3" s="9">
-        <v>3787874</v>
+        <v>4035782</v>
       </c>
       <c r="U3" s="10">
         <f>S3/(S3+T3)</f>
-        <v>0.31704142890936471</v>
+        <v>0.36326868436410442</v>
       </c>
       <c r="V3" s="9">
-        <v>621754931</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>561561179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B4" s="8">
-        <v>9482452</v>
+        <v>20132923</v>
       </c>
       <c r="C4" s="9">
-        <v>20956413</v>
+        <v>15952062</v>
       </c>
       <c r="D4" s="10">
         <f>B4/(B4+C4)</f>
-        <v>0.31152449343955502</v>
+        <v>0.55793075707250539</v>
       </c>
       <c r="E4" s="9">
-        <v>1942745</v>
+        <v>19201200</v>
       </c>
       <c r="F4" s="9">
-        <v>7539707</v>
+        <v>931723</v>
       </c>
       <c r="G4" s="10">
         <f>E4/(E4+F4)</f>
-        <v>0.20487791554336368</v>
+        <v>0.95372142435551954</v>
       </c>
       <c r="H4" s="9">
-        <v>670320719</v>
+        <v>3698781999</v>
       </c>
       <c r="I4" s="9">
-        <v>5508413</v>
+        <v>18865322</v>
       </c>
       <c r="J4" s="9">
-        <v>24930452</v>
+        <v>17219663</v>
       </c>
       <c r="K4" s="10">
         <f>I4/(I4+J4)</f>
-        <v>0.18096643879461341</v>
+        <v>0.52280254515832558</v>
       </c>
       <c r="L4" s="9">
-        <v>1549612</v>
+        <v>18063351</v>
       </c>
       <c r="M4" s="9">
-        <v>3958801</v>
+        <v>801971</v>
       </c>
       <c r="N4" s="10">
         <f>L4/(L4+M4)</f>
-        <v>0.28131732315641544</v>
+        <v>0.95748967338060809</v>
       </c>
       <c r="O4" s="9">
-        <v>452484703</v>
+        <v>3562773747</v>
       </c>
       <c r="P4" s="9">
-        <v>3240984</v>
+        <v>18824301</v>
       </c>
       <c r="Q4" s="9">
-        <v>27197881</v>
+        <v>17260684</v>
       </c>
       <c r="R4" s="10">
         <f>P4/(P4+Q4)</f>
-        <v>0.10647519215976023</v>
+        <v>0.52166575654666336</v>
       </c>
       <c r="S4" s="9">
-        <v>1483242</v>
+        <v>18024023</v>
       </c>
       <c r="T4" s="9">
-        <v>1757742</v>
+        <v>800278</v>
       </c>
       <c r="U4" s="10">
         <f>S4/(S4+T4)</f>
-        <v>0.45765175020919574</v>
+        <v>0.95748697388551107</v>
       </c>
       <c r="V4" s="9">
-        <v>387887513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>3557251525</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="8">
-        <v>14779659</v>
+        <v>10890358</v>
       </c>
       <c r="C5" s="9">
-        <v>15659206</v>
+        <v>24879188</v>
       </c>
       <c r="D5" s="10">
         <f>B5/(B5+C5)</f>
-        <v>0.48555223724669105</v>
+        <v>0.30445893833821652</v>
       </c>
       <c r="E5" s="9">
-        <v>2896191</v>
+        <v>8578628</v>
       </c>
       <c r="F5" s="9">
-        <v>11883468</v>
+        <v>2311730</v>
       </c>
       <c r="G5" s="10">
         <f>E5/(E5+F5)</f>
-        <v>0.19595790403553964</v>
+        <v>0.78772690484555241</v>
       </c>
       <c r="H5" s="9">
-        <v>1184779711</v>
+        <v>1425636583</v>
       </c>
       <c r="I5" s="9">
-        <v>4903099</v>
+        <v>8783659</v>
       </c>
       <c r="J5" s="9">
-        <v>25535766</v>
+        <v>26985887</v>
       </c>
       <c r="K5" s="10">
         <f>I5/(I5+J5)</f>
-        <v>0.16108021767565905</v>
+        <v>0.24556249609653977</v>
       </c>
       <c r="L5" s="9">
-        <v>1474537</v>
+        <v>7183524</v>
       </c>
       <c r="M5" s="9">
-        <v>3428562</v>
+        <v>1600135</v>
       </c>
       <c r="N5" s="10">
         <f>L5/(L5+M5)</f>
-        <v>0.30073571836913754</v>
+        <v>0.81782819665471984</v>
       </c>
       <c r="O5" s="9">
-        <v>389759891</v>
+        <v>1135372173</v>
       </c>
       <c r="P5" s="9">
-        <v>2526847</v>
+        <v>8383020</v>
       </c>
       <c r="Q5" s="9">
-        <v>27912018</v>
+        <v>27386526</v>
       </c>
       <c r="R5" s="10">
         <f>P5/(P5+Q5)</f>
-        <v>8.301383773672244E-2</v>
+        <v>0.23436193459095064</v>
       </c>
       <c r="S5" s="9">
-        <v>1365113</v>
+        <v>6937066</v>
       </c>
       <c r="T5" s="9">
-        <v>1161734</v>
+        <v>1445954</v>
       </c>
       <c r="U5" s="10">
         <f>S5/(S5+T5)</f>
-        <v>0.54024363168802858</v>
+        <v>0.82751395081963297</v>
       </c>
       <c r="V5" s="9">
-        <v>311524099</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8">
-        <v>20443432</v>
-      </c>
-      <c r="C6" s="9">
-        <v>9995433</v>
-      </c>
-      <c r="D6" s="10">
-        <f>B6/(B6+C6)</f>
-        <v>0.67162267712675883</v>
-      </c>
-      <c r="E6" s="9">
-        <v>4663156</v>
-      </c>
-      <c r="F6" s="9">
-        <v>15780276</v>
-      </c>
-      <c r="G6" s="10">
-        <f>E6/(E6+F6)</f>
-        <v>0.22810044810479962</v>
-      </c>
-      <c r="H6" s="9">
-        <v>1970341931</v>
-      </c>
-      <c r="I6" s="9">
-        <v>5176439</v>
-      </c>
-      <c r="J6" s="9">
-        <v>25262426</v>
-      </c>
-      <c r="K6" s="10">
-        <f>I6/(I6+J6)</f>
-        <v>0.17006018456995686</v>
-      </c>
-      <c r="L6" s="9">
-        <v>1515819</v>
-      </c>
-      <c r="M6" s="9">
-        <v>3660620</v>
-      </c>
-      <c r="N6" s="10">
-        <f>L6/(L6+M6)</f>
-        <v>0.29283045738585928</v>
-      </c>
-      <c r="O6" s="9">
-        <v>412603543</v>
-      </c>
-      <c r="P6" s="9">
-        <v>2351529</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>28087336</v>
-      </c>
-      <c r="R6" s="10">
-        <f>P6/(P6+Q6)</f>
-        <v>7.7254161743547267E-2</v>
-      </c>
-      <c r="S6" s="9">
-        <v>1324996</v>
-      </c>
-      <c r="T6" s="9">
-        <v>1026533</v>
-      </c>
-      <c r="U6" s="10">
-        <f>S6/(S6+T6)</f>
-        <v>0.56346147549105285</v>
-      </c>
-      <c r="V6" s="9">
-        <v>291782827</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1087482979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+    </row>
+    <row r="7" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
@@ -2896,7 +4315,7 @@
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
     </row>
-    <row r="8" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -2920,7 +4339,7 @@
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
     </row>
-    <row r="9" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -2944,7 +4363,7 @@
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
     </row>
-    <row r="10" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -2979,478 +4398,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:V10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="22" width="16.33203125" style="15" customWidth="1"/>
-    <col min="23" max="256" width="16.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3"/>
-      <c r="B1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-    </row>
-    <row r="2" spans="1:22" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="16"/>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>9667308</v>
-      </c>
-      <c r="C3" s="9">
-        <v>20771557</v>
-      </c>
-      <c r="D3" s="10">
-        <f>B3/(B3+C3)</f>
-        <v>0.31759751882995635</v>
-      </c>
-      <c r="E3" s="9">
-        <v>3952546</v>
-      </c>
-      <c r="F3" s="9">
-        <v>5714762</v>
-      </c>
-      <c r="G3" s="10">
-        <f>E3/(E3+F3)</f>
-        <v>0.4088569434220985</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1023845511</v>
-      </c>
-      <c r="I3" s="9">
-        <v>6514006</v>
-      </c>
-      <c r="J3" s="9">
-        <v>23924859</v>
-      </c>
-      <c r="K3" s="10">
-        <f>I3/(I3+J3)</f>
-        <v>0.21400292027971476</v>
-      </c>
-      <c r="L3" s="9">
-        <v>2358181</v>
-      </c>
-      <c r="M3" s="9">
-        <v>4155825</v>
-      </c>
-      <c r="N3" s="10">
-        <f>L3/(L3+M3)</f>
-        <v>0.36201701380072415</v>
-      </c>
-      <c r="O3" s="9">
-        <v>576070403</v>
-      </c>
-      <c r="P3" s="9">
-        <v>6338281</v>
-      </c>
-      <c r="Q3" s="9">
-        <v>24100584</v>
-      </c>
-      <c r="R3" s="10">
-        <f>P3/(P3+Q3)</f>
-        <v>0.2082298732229339</v>
-      </c>
-      <c r="S3" s="9">
-        <v>2302499</v>
-      </c>
-      <c r="T3" s="9">
-        <v>4035782</v>
-      </c>
-      <c r="U3" s="10">
-        <f>S3/(S3+T3)</f>
-        <v>0.36326868436410442</v>
-      </c>
-      <c r="V3" s="9">
-        <v>561561179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="8">
-        <v>20132923</v>
-      </c>
-      <c r="C4" s="9">
-        <v>15952062</v>
-      </c>
-      <c r="D4" s="10">
-        <f>B4/(B4+C4)</f>
-        <v>0.55793075707250539</v>
-      </c>
-      <c r="E4" s="9">
-        <v>19201200</v>
-      </c>
-      <c r="F4" s="9">
-        <v>931723</v>
-      </c>
-      <c r="G4" s="10">
-        <f>E4/(E4+F4)</f>
-        <v>0.95372142435551954</v>
-      </c>
-      <c r="H4" s="9">
-        <v>3698781999</v>
-      </c>
-      <c r="I4" s="9">
-        <v>18865322</v>
-      </c>
-      <c r="J4" s="9">
-        <v>17219663</v>
-      </c>
-      <c r="K4" s="10">
-        <f>I4/(I4+J4)</f>
-        <v>0.52280254515832558</v>
-      </c>
-      <c r="L4" s="9">
-        <v>18063351</v>
-      </c>
-      <c r="M4" s="9">
-        <v>801971</v>
-      </c>
-      <c r="N4" s="10">
-        <f>L4/(L4+M4)</f>
-        <v>0.95748967338060809</v>
-      </c>
-      <c r="O4" s="9">
-        <v>3562773747</v>
-      </c>
-      <c r="P4" s="9">
-        <v>18824301</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>17260684</v>
-      </c>
-      <c r="R4" s="10">
-        <f>P4/(P4+Q4)</f>
-        <v>0.52166575654666336</v>
-      </c>
-      <c r="S4" s="9">
-        <v>18024023</v>
-      </c>
-      <c r="T4" s="9">
-        <v>800278</v>
-      </c>
-      <c r="U4" s="10">
-        <f>S4/(S4+T4)</f>
-        <v>0.95748697388551107</v>
-      </c>
-      <c r="V4" s="9">
-        <v>3557251525</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="8">
-        <v>10890358</v>
-      </c>
-      <c r="C5" s="9">
-        <v>24879188</v>
-      </c>
-      <c r="D5" s="10">
-        <f>B5/(B5+C5)</f>
-        <v>0.30445893833821652</v>
-      </c>
-      <c r="E5" s="9">
-        <v>8578628</v>
-      </c>
-      <c r="F5" s="9">
-        <v>2311730</v>
-      </c>
-      <c r="G5" s="10">
-        <f>E5/(E5+F5)</f>
-        <v>0.78772690484555241</v>
-      </c>
-      <c r="H5" s="9">
-        <v>1425636583</v>
-      </c>
-      <c r="I5" s="9">
-        <v>8783659</v>
-      </c>
-      <c r="J5" s="9">
-        <v>26985887</v>
-      </c>
-      <c r="K5" s="10">
-        <f>I5/(I5+J5)</f>
-        <v>0.24556249609653977</v>
-      </c>
-      <c r="L5" s="9">
-        <v>7183524</v>
-      </c>
-      <c r="M5" s="9">
-        <v>1600135</v>
-      </c>
-      <c r="N5" s="10">
-        <f>L5/(L5+M5)</f>
-        <v>0.81782819665471984</v>
-      </c>
-      <c r="O5" s="9">
-        <v>1135372173</v>
-      </c>
-      <c r="P5" s="9">
-        <v>8383020</v>
-      </c>
-      <c r="Q5" s="9">
-        <v>27386526</v>
-      </c>
-      <c r="R5" s="10">
-        <f>P5/(P5+Q5)</f>
-        <v>0.23436193459095064</v>
-      </c>
-      <c r="S5" s="9">
-        <v>6937066</v>
-      </c>
-      <c r="T5" s="9">
-        <v>1445954</v>
-      </c>
-      <c r="U5" s="10">
-        <f>S5/(S5+T5)</f>
-        <v>0.82751395081963297</v>
-      </c>
-      <c r="V5" s="9">
-        <v>1087482979</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-    </row>
-    <row r="7" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-    </row>
-    <row r="8" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-    </row>
-    <row r="9" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-    </row>
-    <row r="10" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="B1:H1"/>
-  </mergeCells>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>